<commit_message>
Atnaujinta NPD formulė (įsigaliojusi nuo 2020-07-01)
</commit_message>
<xml_diff>
--- a/2020/atlyginimai2020.xlsx
+++ b/2020/atlyginimai2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irenata\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4830DCF-90EE-408B-B665-0CAE9BA44CE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D548A761-D205-4FDD-A3C4-FE0DCBB46676}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="-120" windowWidth="28515" windowHeight="16440" xr2:uid="{71DF866D-CBC4-40B7-8D66-9127891468C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{71DF866D-CBC4-40B7-8D66-9127891468C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -330,6 +324,22 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -338,22 +348,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -376,7 +370,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,7 +386,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="„Office“ tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -694,7 +688,7 @@
   <dimension ref="A3:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +719,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -746,7 +740,7 @@
       <c r="G3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="21" t="s">
@@ -779,19 +773,19 @@
         <v>15</v>
       </c>
       <c r="V3" s="29"/>
-      <c r="W3" s="19" t="s">
+      <c r="W3" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="22"/>
       <c r="J4" s="14" t="s">
         <v>4</v>
@@ -824,7 +818,7 @@
       <c r="V4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="20"/>
+      <c r="W4" s="24"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -876,12 +870,12 @@
         <v>17.7</v>
       </c>
       <c r="P5" s="11">
-        <f>ROUND(IF(G5="taip",(IF(AND(N5&lt;=607,N5&gt;=350),350,(IF(N5&lt;350,N5,IF(350-0.17*(N5-607)&lt;0,0,(350-0.17*(N5-607))))))),0),2)</f>
-        <v>283.19</v>
+        <f>ROUND(IF(G5="taip",(IF(AND(N5&lt;=607,N5&gt;=400),400,(IF(N5&lt;400,N5,IF(400-0.19*(N5-607)&lt;0,0,(400-0.19*(N5-607))))))),0),2)</f>
+        <v>325.33</v>
       </c>
       <c r="Q5" s="11">
         <f t="shared" ref="Q5:Q14" si="0">ROUND(((N5-P5-H5-M5)*0.2)+(M5*0.15),2)</f>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R5" s="11">
         <f>ROUND((N5-M5)*(0.195+(I5/100)),2)</f>
@@ -903,7 +897,7 @@
       </c>
       <c r="W5" s="11">
         <f>ROUND(N5-Q5-R5-U5-V5,2)</f>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -956,12 +950,12 @@
         <v>17.7</v>
       </c>
       <c r="P6" s="11">
-        <f t="shared" ref="P6:P14" si="4">ROUND(IF(G6="taip",(IF(AND(N6&lt;=607,N6&gt;=350),350,(IF(N6&lt;350,N6,IF(350-0.17*(N6-607)&lt;0,0,(350-0.17*(N6-607))))))),0),2)</f>
-        <v>283.19</v>
+        <f t="shared" ref="P6:P14" si="4">ROUND(IF(G6="taip",(IF(AND(N6&lt;=607,N6&gt;=400),400,(IF(N6&lt;400,N6,IF(400-0.19*(N6-607)&lt;0,0,(400-0.19*(N6-607))))))),0),2)</f>
+        <v>325.33</v>
       </c>
       <c r="Q6" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R6" s="11">
         <f t="shared" ref="R6:R14" si="5">ROUND((N6-M6)*(0.195+(I6/100)),2)</f>
@@ -983,7 +977,7 @@
       </c>
       <c r="W6" s="11">
         <f t="shared" ref="W6:W14" si="8">ROUND(N6-Q6-R6-U6-V6,2)</f>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1037,11 +1031,11 @@
       </c>
       <c r="P7" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q7" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R7" s="11">
         <f t="shared" si="5"/>
@@ -1063,7 +1057,7 @@
       </c>
       <c r="W7" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1117,11 +1111,11 @@
       </c>
       <c r="P8" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q8" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R8" s="11">
         <f t="shared" si="5"/>
@@ -1143,7 +1137,7 @@
       </c>
       <c r="W8" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1197,11 +1191,11 @@
       </c>
       <c r="P9" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q9" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R9" s="11">
         <f t="shared" si="5"/>
@@ -1223,7 +1217,7 @@
       </c>
       <c r="W9" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1277,11 +1271,11 @@
       </c>
       <c r="P10" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q10" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R10" s="11">
         <f t="shared" si="5"/>
@@ -1303,7 +1297,7 @@
       </c>
       <c r="W10" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1357,11 +1351,11 @@
       </c>
       <c r="P11" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q11" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R11" s="11">
         <f t="shared" si="5"/>
@@ -1383,7 +1377,7 @@
       </c>
       <c r="W11" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1437,11 +1431,11 @@
       </c>
       <c r="P12" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q12" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R12" s="11">
         <f t="shared" si="5"/>
@@ -1463,7 +1457,7 @@
       </c>
       <c r="W12" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1517,11 +1511,11 @@
       </c>
       <c r="P13" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q13" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R13" s="11">
         <f t="shared" si="5"/>
@@ -1543,7 +1537,7 @@
       </c>
       <c r="W13" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1597,11 +1591,11 @@
       </c>
       <c r="P14" s="11">
         <f t="shared" si="4"/>
-        <v>283.19</v>
+        <v>325.33</v>
       </c>
       <c r="Q14" s="11">
         <f t="shared" si="0"/>
-        <v>143.36000000000001</v>
+        <v>134.93</v>
       </c>
       <c r="R14" s="11">
         <f t="shared" si="5"/>
@@ -1623,7 +1617,7 @@
       </c>
       <c r="W14" s="11">
         <f t="shared" si="8"/>
-        <v>661.64</v>
+        <v>670.07</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1664,11 +1658,11 @@
       </c>
       <c r="P15" s="17">
         <f t="shared" si="9"/>
-        <v>2831.9</v>
+        <v>3253.2999999999997</v>
       </c>
       <c r="Q15" s="17">
         <f t="shared" si="9"/>
-        <v>1433.6000000000004</v>
+        <v>1349.3000000000004</v>
       </c>
       <c r="R15" s="17">
         <f t="shared" si="9"/>
@@ -1689,7 +1683,7 @@
       </c>
       <c r="W15" s="17">
         <f>SUM(W5:W14)</f>
-        <v>6616.4000000000005</v>
+        <v>6700.7</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -1753,12 +1747,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="17">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D3:D4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
@@ -1770,6 +1758,12 @@
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="O3:O4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I14" xr:uid="{37C88D5E-F204-411F-81CC-1124D2BC86F0}">

</xml_diff>